<commit_message>
Sample data: add category with dataset
</commit_message>
<xml_diff>
--- a/lib/csc_core/samples/assets/csv/primary_schools.xlsx
+++ b/lib/csc_core/samples/assets/csv/primary_schools.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/www/csc-web/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/www/csc-webportal/engines/csc_core/lib/csc_core/samples/assets/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Koh Kong" sheetId="1" r:id="rId1"/>
@@ -110,18 +110,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
-    <t>commune_code</t>
-  </si>
-  <si>
-    <t>school_code</t>
-  </si>
-  <si>
-    <t>school_name_en</t>
-  </si>
-  <si>
-    <t>school_name_km</t>
-  </si>
-  <si>
     <t>090101</t>
   </si>
   <si>
@@ -180,6 +168,18 @@
   </si>
   <si>
     <t>ឆ្លូង</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>name_en</t>
+  </si>
+  <si>
+    <t>name_km</t>
   </si>
 </sst>
 </file>
@@ -505,8 +505,8 @@
   </sheetPr>
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -519,16 +519,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -552,45 +552,45 @@
     </row>
     <row r="2" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -606,9 +606,7 @@
   </sheetPr>
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -620,16 +618,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -653,44 +651,44 @@
     </row>
     <row r="2" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>